<commit_message>
Integrating Tim's moving FFT code
</commit_message>
<xml_diff>
--- a/Docs/CITEPH/TestNotes_LB.xlsx
+++ b/Docs/CITEPH/TestNotes_LB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="1700" windowWidth="25600" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="81">
   <si>
     <t xml:space="preserve">Oceanide/CITEPH July 2013 </t>
   </si>
@@ -259,13 +259,16 @@
   </si>
   <si>
     <t>Floes not very dynamic. Strong attn. From OW? Scattering doesn't look that strong. Scattering is strong enough that floe motions are complicated when excited.</t>
+  </si>
+  <si>
+    <t>Single floe tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -318,8 +321,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +360,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4BD97"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -359,7 +376,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -396,8 +413,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,7 +447,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="31" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,24 +471,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="31" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="42">
     <cellStyle name="Bad" xfId="31" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -468,6 +503,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -485,6 +523,9 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -814,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47:R47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -827,72 +868,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="T1" s="17" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="T1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="17"/>
+      <c r="U1" s="13"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
       <c r="T3" t="s">
         <v>7</v>
       </c>
@@ -909,18 +950,18 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="T5" t="s">
         <v>15</v>
       </c>
@@ -929,16 +970,16 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
       <c r="T6" t="s">
         <v>16</v>
       </c>
@@ -947,22 +988,22 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="T8" s="17" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="T8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="17"/>
+      <c r="U8" s="13"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
     </row>
     <row r="10" spans="1:21">
       <c r="T10">
@@ -1003,16 +1044,16 @@
       <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
       <c r="T11">
         <v>0.8</v>
       </c>
@@ -1680,11 +1721,11 @@
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
       <c r="R26" s="12"/>
-      <c r="S26" s="15" t="s">
+      <c r="S26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="5">
@@ -1729,9 +1770,9 @@
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="5">
@@ -1766,19 +1807,19 @@
       <c r="J28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="5">
@@ -1813,19 +1854,19 @@
       <c r="J29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="5">
@@ -1860,19 +1901,19 @@
       <c r="J30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="5">
@@ -1907,19 +1948,19 @@
       <c r="J31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K31" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="18"/>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="5">
@@ -1954,19 +1995,19 @@
       <c r="J32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="5">
@@ -2001,19 +2042,19 @@
       <c r="J33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="5">
@@ -2048,19 +2089,19 @@
       <c r="J34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="5">
@@ -2095,19 +2136,19 @@
       <c r="J35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="5">
@@ -2142,19 +2183,19 @@
       <c r="J36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
+      <c r="U36" s="18"/>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1"/>
@@ -2175,16 +2216,16 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
     </row>
     <row r="38" spans="1:21" ht="15" customHeight="1">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2200,14 +2241,14 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2223,9 +2264,9 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1"/>
@@ -2246,9 +2287,9 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="3" t="s">
@@ -2281,16 +2322,16 @@
       <c r="J41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="K41" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="5">
@@ -2325,16 +2366,16 @@
       <c r="J42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="K42" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="5">
@@ -2369,16 +2410,16 @@
       <c r="J43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="9" t="s">
+      <c r="K43" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="5">
@@ -2413,16 +2454,16 @@
       <c r="J44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="K44" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="5">
@@ -2457,16 +2498,16 @@
       <c r="J45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K45" s="9" t="s">
+      <c r="K45" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="5">
@@ -2501,16 +2542,16 @@
       <c r="J46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K46" s="9" t="s">
+      <c r="K46" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="5">
@@ -2545,22 +2586,22 @@
       <c r="J47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K47" s="9" t="s">
+      <c r="K47" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="5">
         <v>41480</v>
       </c>
-      <c r="B48" s="16"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="1">
         <v>0.39</v>
       </c>
@@ -2578,25 +2619,25 @@
         <f t="shared" si="2"/>
         <v>1.3071041108424286</v>
       </c>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="9" t="s">
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="5">
         <v>41480</v>
       </c>
-      <c r="B49" s="16"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="1">
         <v>0.39</v>
       </c>
@@ -2614,19 +2655,19 @@
         <f t="shared" si="2"/>
         <v>0.64049189777749316</v>
       </c>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="9" t="s">
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
@@ -2649,9 +2690,11 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2669,9 +2712,9 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2689,51 +2732,79 @@
       <c r="R52" s="1"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
+      <c r="A54" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D55" s="4">
+        <v>20</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0.65</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2749,11 +2820,17 @@
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D56" s="4">
+        <v>30</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.95</v>
+      </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -2769,11 +2846,17 @@
       <c r="R56" s="1"/>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D57" s="4">
+        <v>40</v>
+      </c>
+      <c r="E57" s="4">
+        <v>1.25</v>
+      </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -2789,11 +2872,17 @@
       <c r="R57" s="1"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D58" s="4">
+        <v>40</v>
+      </c>
+      <c r="E58" s="4">
+        <v>1.55</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -2809,11 +2898,17 @@
       <c r="R58" s="1"/>
     </row>
     <row r="59" spans="1:18">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D59" s="4">
+        <v>40</v>
+      </c>
+      <c r="E59" s="4">
+        <v>1.85</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -2828,18 +2923,41 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
+    <row r="60" spans="1:18">
+      <c r="A60" s="5"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D60" s="4">
+        <v>80</v>
+      </c>
+      <c r="E60" s="4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="5"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="D61" s="4">
+        <v>60</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="K47:R47"/>
-    <mergeCell ref="K48:R48"/>
-    <mergeCell ref="K49:R49"/>
-    <mergeCell ref="K27:R27"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="K16:R16"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="K23:R23"/>
+  <mergeCells count="43">
+    <mergeCell ref="A51:C52"/>
+    <mergeCell ref="K54:R54"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="K41:R41"/>
+    <mergeCell ref="K42:R42"/>
+    <mergeCell ref="K43:R43"/>
+    <mergeCell ref="K44:R44"/>
     <mergeCell ref="T1:U2"/>
     <mergeCell ref="K24:R24"/>
     <mergeCell ref="K25:R25"/>
@@ -2856,15 +2974,20 @@
     <mergeCell ref="K35:R35"/>
     <mergeCell ref="K36:R36"/>
     <mergeCell ref="K18:R18"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="K23:R23"/>
     <mergeCell ref="K19:R19"/>
     <mergeCell ref="K20:R20"/>
     <mergeCell ref="K21:R21"/>
     <mergeCell ref="K22:R22"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="K41:R41"/>
-    <mergeCell ref="K42:R42"/>
-    <mergeCell ref="K43:R43"/>
-    <mergeCell ref="K44:R44"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="K47:R47"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="K49:R49"/>
+    <mergeCell ref="K27:R27"/>
     <mergeCell ref="K45:R45"/>
     <mergeCell ref="K28:R28"/>
     <mergeCell ref="K29:R29"/>

</xml_diff>

<commit_message>
Modifications to Main_WaveData & MovingFFT + some small extra additions
</commit_message>
<xml_diff>
--- a/Docs/CITEPH/TestNotes_LB.xlsx
+++ b/Docs/CITEPH/TestNotes_LB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1700" windowWidth="25600" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="86">
   <si>
     <t xml:space="preserve">Oceanide/CITEPH July 2013 </t>
   </si>
@@ -262,6 +262,21 @@
   </si>
   <si>
     <t>Single floe tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floe moves with waves as expected. Nb. nonlin waves, generated by WM, present after ~1min &amp; cause scattering (perhaps affect drift). </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Repeat of previous test, due to problems with recording devices. Very similar behaviour to prev test. Non-lin after ~5-10 cycles. Not much evidence of reflect waves from BCH.</t>
+  </si>
+  <si>
+    <t>Two (repeated) tests pushing the floe were conducted to test the restoring force and drag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to prev expt. More pitching. Slight scattering from linear waves. Again, eventually corrupted by non-lin waves from WM. </t>
   </si>
 </sst>
 </file>
@@ -376,7 +391,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -419,8 +434,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,39 +485,42 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="31" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="60">
     <cellStyle name="Bad" xfId="31" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -506,6 +542,15 @@
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -526,6 +571,15 @@
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -855,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="K42" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57:R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,72 +922,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="T1" s="13" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="T1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="13"/>
+      <c r="U1" s="17"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
       <c r="T3" t="s">
         <v>7</v>
       </c>
@@ -950,18 +1004,18 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
       <c r="T5" t="s">
         <v>15</v>
       </c>
@@ -970,16 +1024,16 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
       <c r="T6" t="s">
         <v>16</v>
       </c>
@@ -988,22 +1042,22 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="T8" s="13" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="T8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="13"/>
+      <c r="U8" s="17"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21">
       <c r="T10">
@@ -1044,16 +1098,16 @@
       <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
       <c r="T11">
         <v>0.8</v>
       </c>
@@ -1101,16 +1155,16 @@
       <c r="J13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
       <c r="T13">
         <v>1.1000000000000001</v>
       </c>
@@ -1150,16 +1204,16 @@
       <c r="J14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
       <c r="T14">
         <v>1.25</v>
       </c>
@@ -1199,16 +1253,16 @@
       <c r="J15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
       <c r="T15">
         <v>1.4</v>
       </c>
@@ -1248,16 +1302,16 @@
       <c r="J16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
       <c r="T16">
         <v>1.55</v>
       </c>
@@ -1297,16 +1351,16 @@
       <c r="J17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
       <c r="T17">
         <v>1.7</v>
       </c>
@@ -1347,16 +1401,16 @@
       <c r="J18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
       <c r="T18">
         <v>1.85</v>
       </c>
@@ -1397,16 +1451,16 @@
       <c r="J19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
       <c r="T19">
         <v>2</v>
       </c>
@@ -1447,16 +1501,16 @@
       <c r="J20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="5">
@@ -1491,16 +1545,16 @@
       <c r="J21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="5">
@@ -1535,16 +1589,16 @@
       <c r="J22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="5">
@@ -1579,16 +1633,16 @@
       <c r="J23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="5">
@@ -1623,16 +1677,16 @@
       <c r="J24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="5">
@@ -1667,16 +1721,16 @@
       <c r="J25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="5">
@@ -1711,21 +1765,21 @@
       <c r="J26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="18" t="s">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="5">
@@ -1760,19 +1814,19 @@
       <c r="J27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="K27" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="5">
@@ -1807,19 +1861,19 @@
       <c r="J28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="5">
@@ -1854,19 +1908,19 @@
       <c r="J29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="5">
@@ -1901,19 +1955,19 @@
       <c r="J30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="5">
@@ -1948,19 +2002,19 @@
       <c r="J31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="5">
@@ -1995,19 +2049,19 @@
       <c r="J32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="5">
@@ -2042,19 +2096,19 @@
       <c r="J33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="5">
@@ -2089,19 +2143,19 @@
       <c r="J34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="5">
@@ -2136,19 +2190,19 @@
       <c r="J35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="U35" s="18"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="5">
@@ -2183,19 +2237,19 @@
       <c r="J36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K36" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1"/>
@@ -2216,16 +2270,16 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
     </row>
     <row r="38" spans="1:21" ht="15" customHeight="1">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2241,14 +2295,14 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2264,9 +2318,9 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1"/>
@@ -2287,9 +2341,9 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="3" t="s">
@@ -2322,16 +2376,16 @@
       <c r="J41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="17" t="s">
+      <c r="K41" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="5">
@@ -2366,16 +2420,16 @@
       <c r="J42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K42" s="11" t="s">
+      <c r="K42" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="5">
@@ -2410,16 +2464,16 @@
       <c r="J43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="K43" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="5">
@@ -2454,16 +2508,16 @@
       <c r="J44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K44" s="11" t="s">
+      <c r="K44" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="5">
@@ -2498,16 +2552,16 @@
       <c r="J45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="K45" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="5">
@@ -2542,16 +2596,16 @@
       <c r="J46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K46" s="11" t="s">
+      <c r="K46" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="5">
@@ -2586,16 +2640,16 @@
       <c r="J47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K47" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="5">
@@ -2622,16 +2676,16 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="11" t="s">
+      <c r="K48" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="5">
@@ -2658,16 +2712,16 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="11" t="s">
+      <c r="K49" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
@@ -2690,11 +2744,11 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2712,9 +2766,9 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2752,212 +2806,411 @@
       <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H54" s="19" t="s">
+      <c r="H54" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I54" s="19" t="s">
+      <c r="I54" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="19" t="s">
+      <c r="J54" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K54" s="20" t="s">
+      <c r="K54" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-      <c r="O54" s="20"/>
-      <c r="P54" s="20"/>
-      <c r="Q54" s="20"/>
-      <c r="R54" s="20"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="5"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="4">
-        <v>0.39</v>
+      <c r="A55" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B55" s="8">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D55" s="4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E55" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="F55" s="4">
+        <f>U18</f>
+        <v>5.3436000000000003</v>
+      </c>
+      <c r="G55" s="4">
+        <f>D55/F55/10</f>
+        <v>0.74855902387903284</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K55" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="22"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="5"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="4">
-        <v>0.39</v>
+      <c r="A56" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B56" s="8">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D56" s="4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E56" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="F56" s="4">
+        <f>F55</f>
+        <v>5.3436000000000003</v>
+      </c>
+      <c r="G56" s="4">
+        <f>D56/F56/10</f>
+        <v>0.74855902387903284</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K56" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="22"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="22"/>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57" s="5"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="4">
-        <v>0.39</v>
+      <c r="A57" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B57" s="8">
+        <v>0.51111111111111118</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D57" s="4">
         <v>40</v>
       </c>
       <c r="E57" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
+        <v>1.55</v>
+      </c>
+      <c r="F57" s="4">
+        <f>F31</f>
+        <v>3.7509999999999999</v>
+      </c>
+      <c r="G57" s="4">
+        <f t="shared" ref="G57:G62" si="3">D57/F57/10</f>
+        <v>1.0663822980538522</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K57" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="22"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="5"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="4">
-        <v>0.39</v>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D58" s="4">
         <v>40</v>
       </c>
       <c r="E58" s="4">
-        <v>1.55</v>
-      </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="F58" s="4">
+        <f>F30</f>
+        <v>2.4394999999999998</v>
+      </c>
+      <c r="G58" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6396802623488422</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="5"/>
       <c r="B59" s="8"/>
-      <c r="C59" s="4">
-        <v>0.39</v>
+      <c r="C59" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D59" s="4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E59" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F59" s="1">
+        <f>F29</f>
+        <v>1.4091</v>
+      </c>
+      <c r="G59" s="4">
+        <f t="shared" si="3"/>
+        <v>2.1290185224611453</v>
+      </c>
       <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
+      <c r="I59" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="5"/>
       <c r="B60" s="8"/>
-      <c r="C60" s="4">
-        <v>0.39</v>
+      <c r="C60" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D60" s="4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E60" s="4">
-        <v>1.25</v>
-      </c>
+        <v>0.65</v>
+      </c>
+      <c r="F60" s="4">
+        <f>F28</f>
+        <v>0.65969999999999995</v>
+      </c>
+      <c r="G60" s="4">
+        <f t="shared" si="3"/>
+        <v>3.031681067151736</v>
+      </c>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="5"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="4">
-        <v>0.39</v>
+      <c r="C61" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D61" s="4">
+        <v>80</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="F61" s="4">
+        <f>F58</f>
+        <v>2.4394999999999998</v>
+      </c>
+      <c r="G61" s="4">
+        <f t="shared" si="3"/>
+        <v>3.2793605246976845</v>
+      </c>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="C62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="4">
         <v>60</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E62" s="4">
         <v>0.95</v>
       </c>
+      <c r="F62" s="4">
+        <f>F59</f>
+        <v>1.4091</v>
+      </c>
+      <c r="G62" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2580370449222906</v>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="22"/>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" s="5"/>
+      <c r="B63" s="8"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="22"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="22"/>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="A64" s="5"/>
+      <c r="B64" s="8">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="K64" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="22"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="A51:C52"/>
-    <mergeCell ref="K54:R54"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="K41:R41"/>
-    <mergeCell ref="K42:R42"/>
-    <mergeCell ref="K43:R43"/>
-    <mergeCell ref="K44:R44"/>
+  <mergeCells count="53">
+    <mergeCell ref="K61:R61"/>
+    <mergeCell ref="K62:R62"/>
+    <mergeCell ref="K63:R63"/>
+    <mergeCell ref="K64:R64"/>
+    <mergeCell ref="K56:R56"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K57:R57"/>
+    <mergeCell ref="K58:R58"/>
+    <mergeCell ref="K59:R59"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="K27:R27"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="K29:R29"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K31:R31"/>
+    <mergeCell ref="K34:R34"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="K22:R22"/>
     <mergeCell ref="T1:U2"/>
     <mergeCell ref="K24:R24"/>
     <mergeCell ref="K25:R25"/>
@@ -2974,26 +3227,17 @@
     <mergeCell ref="K35:R35"/>
     <mergeCell ref="K36:R36"/>
     <mergeCell ref="K18:R18"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="K16:R16"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="K23:R23"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="K20:R20"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="A51:C52"/>
+    <mergeCell ref="K54:R54"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="K41:R41"/>
+    <mergeCell ref="K42:R42"/>
+    <mergeCell ref="K43:R43"/>
+    <mergeCell ref="K44:R44"/>
     <mergeCell ref="K46:R46"/>
     <mergeCell ref="K47:R47"/>
     <mergeCell ref="K48:R48"/>
     <mergeCell ref="K49:R49"/>
-    <mergeCell ref="K27:R27"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="K29:R29"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K31:R31"/>
-    <mergeCell ref="K34:R34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Created v1 of single disk analysis functions & moved Main_WaveData -> Main_AttnData
</commit_message>
<xml_diff>
--- a/Docs/CITEPH/TestNotes_LB.xlsx
+++ b/Docs/CITEPH/TestNotes_LB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
   <si>
     <t xml:space="preserve">Oceanide/CITEPH July 2013 </t>
   </si>
@@ -277,6 +277,33 @@
   </si>
   <si>
     <t xml:space="preserve">Similar to prev expt. More pitching. Slight scattering from linear waves. Again, eventually corrupted by non-lin waves from WM. </t>
+  </si>
+  <si>
+    <t>More of the same. Pronounced scattering with from and rear lobes -&gt; does this come from the pitching? Close to onset of OW.</t>
+  </si>
+  <si>
+    <t>Repeat of prev test but with 100 periods to help calculate drift</t>
+  </si>
+  <si>
+    <t>Scatterered waves significant (may be picked up by probes). OW beginning (100mm at front of floe). Is the `high fre' appearance of circ waves due to phase mismatch of angular modes?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OW gradually builds up from WM side of floe till front of floe is weighted down &amp; OW flow  begins. Scattering strong - partic ref (from OW?). </t>
+  </si>
+  <si>
+    <t>OW from front &amp; back. Motion less `smooth' than other prev tests (OW or higher amp???). Circ scat waves significant.</t>
+  </si>
+  <si>
+    <t>OW &amp; scattering strong. Is the period of the oscillations that of the wave? OW may perturb this.</t>
+  </si>
+  <si>
+    <t>1 to 1.5</t>
+  </si>
+  <si>
+    <t>1 to 3.5</t>
   </si>
 </sst>
 </file>
@@ -488,35 +515,35 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K42" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57:R57"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -922,72 +949,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="T1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="T1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="17"/>
+      <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
       <c r="T3" t="s">
         <v>7</v>
       </c>
@@ -1004,18 +1031,18 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
       <c r="T5" t="s">
         <v>15</v>
       </c>
@@ -1024,16 +1051,16 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
       <c r="T6" t="s">
         <v>16</v>
       </c>
@@ -1042,22 +1069,22 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="T8" s="17" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="T8" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="17"/>
+      <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:21">
       <c r="T10">
@@ -1098,16 +1125,16 @@
       <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
       <c r="T11">
         <v>0.8</v>
       </c>
@@ -1155,16 +1182,16 @@
       <c r="J13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
       <c r="T13">
         <v>1.1000000000000001</v>
       </c>
@@ -1195,8 +1222,8 @@
         <f t="shared" ref="G14:G31" si="0">D14/F14/10</f>
         <v>2.0016012810248198</v>
       </c>
-      <c r="H14" s="1">
-        <v>3.5</v>
+      <c r="H14" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>22</v>
@@ -1204,16 +1231,16 @@
       <c r="J14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
       <c r="T14">
         <v>1.25</v>
       </c>
@@ -1244,8 +1271,8 @@
         <f t="shared" si="0"/>
         <v>4.0032025620496396</v>
       </c>
-      <c r="H15" s="1">
-        <v>1.5</v>
+      <c r="H15" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>45</v>
@@ -1253,16 +1280,16 @@
       <c r="J15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
       <c r="T15">
         <v>1.4</v>
       </c>
@@ -1302,16 +1329,16 @@
       <c r="J16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
       <c r="T16">
         <v>1.55</v>
       </c>
@@ -1319,7 +1346,7 @@
         <v>3.7509999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" s="5">
         <v>41478</v>
       </c>
@@ -1351,16 +1378,16 @@
       <c r="J17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
       <c r="T17">
         <v>1.7</v>
       </c>
@@ -1368,7 +1395,7 @@
         <v>4.5122</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" s="5">
         <v>41479</v>
       </c>
@@ -1401,16 +1428,16 @@
       <c r="J18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
       <c r="T18">
         <v>1.85</v>
       </c>
@@ -1418,7 +1445,7 @@
         <v>5.3436000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" s="5">
         <v>41479</v>
       </c>
@@ -1451,16 +1478,16 @@
       <c r="J19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
       <c r="T19">
         <v>2</v>
       </c>
@@ -1468,7 +1495,7 @@
         <v>6.2451999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="A20" s="5">
         <v>41479</v>
       </c>
@@ -1501,18 +1528,18 @@
       <c r="J20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="5">
         <v>41479</v>
       </c>
@@ -1545,18 +1572,18 @@
       <c r="J21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="5">
         <v>41479</v>
       </c>
@@ -1589,18 +1616,18 @@
       <c r="J22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="5">
         <v>41479</v>
       </c>
@@ -1633,18 +1660,18 @@
       <c r="J23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="5">
         <v>41479</v>
       </c>
@@ -1677,18 +1704,18 @@
       <c r="J24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="5">
         <v>41479</v>
       </c>
@@ -1721,18 +1748,18 @@
       <c r="J25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="5">
         <v>41479</v>
       </c>
@@ -1765,23 +1792,24 @@
       <c r="J26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K26" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="21" t="s">
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="5">
         <v>41479</v>
       </c>
@@ -1814,21 +1842,22 @@
       <c r="J27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="5">
         <v>41480</v>
       </c>
@@ -1861,21 +1890,22 @@
       <c r="J28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="5">
         <v>41480</v>
       </c>
@@ -1908,21 +1938,22 @@
       <c r="J29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="16" t="s">
+      <c r="K29" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="5">
         <v>41480</v>
       </c>
@@ -1955,21 +1986,22 @@
       <c r="J30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="16" t="s">
+      <c r="K30" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="21"/>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="5">
         <v>41480</v>
       </c>
@@ -2002,21 +2034,22 @@
       <c r="J31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="5">
         <v>41480</v>
       </c>
@@ -2049,21 +2082,22 @@
       <c r="J32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="16" t="s">
+      <c r="K32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="5">
         <v>41480</v>
       </c>
@@ -2096,21 +2130,22 @@
       <c r="J33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K33" s="16" t="s">
+      <c r="K33" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="5">
         <v>41480</v>
       </c>
@@ -2143,21 +2178,22 @@
       <c r="J34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="5">
         <v>41480</v>
       </c>
@@ -2190,21 +2226,22 @@
       <c r="J35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="16" t="s">
+      <c r="K35" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="5">
         <v>41480</v>
       </c>
@@ -2237,21 +2274,22 @@
       <c r="J36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="16" t="s">
+      <c r="K36" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2270,16 +2308,17 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-    </row>
-    <row r="38" spans="1:21" ht="15" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="12"/>
+    </row>
+    <row r="38" spans="1:22" ht="15" customHeight="1">
+      <c r="A38" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2295,14 +2334,15 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
-    </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+    </row>
+    <row r="39" spans="1:22" ht="15" customHeight="1">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2318,11 +2358,12 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2341,11 +2382,12 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
@@ -2376,18 +2418,18 @@
       <c r="J41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="5">
         <v>41479</v>
       </c>
@@ -2420,18 +2462,18 @@
       <c r="J42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K42" s="16" t="s">
+      <c r="K42" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" s="5">
         <v>41479</v>
       </c>
@@ -2464,18 +2506,18 @@
       <c r="J43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="16" t="s">
+      <c r="K43" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="5">
         <v>41479</v>
       </c>
@@ -2508,18 +2550,18 @@
       <c r="J44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K44" s="16" t="s">
+      <c r="K44" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="5">
         <v>41479</v>
       </c>
@@ -2552,18 +2594,18 @@
       <c r="J45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K45" s="16" t="s">
+      <c r="K45" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16"/>
-      <c r="R45" s="16"/>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" s="5">
         <v>41480</v>
       </c>
@@ -2596,18 +2638,18 @@
       <c r="J46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K46" s="16" t="s">
+      <c r="K46" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="L46" s="16"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="16"/>
-      <c r="O46" s="16"/>
-      <c r="P46" s="16"/>
-      <c r="Q46" s="16"/>
-      <c r="R46" s="16"/>
-    </row>
-    <row r="47" spans="1:21">
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="5">
         <v>41480</v>
       </c>
@@ -2640,18 +2682,18 @@
       <c r="J47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K47" s="16" t="s">
+      <c r="K47" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
-    </row>
-    <row r="48" spans="1:21">
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="5">
         <v>41480</v>
       </c>
@@ -2676,16 +2718,16 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="16" t="s">
+      <c r="K48" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="5">
@@ -2712,16 +2754,16 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="16" t="s">
+      <c r="K49" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="16"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
@@ -2744,11 +2786,11 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2766,9 +2808,9 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2836,16 +2878,16 @@
       <c r="J54" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K54" s="14" t="s">
+      <c r="K54" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="22"/>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="5">
@@ -2880,16 +2922,16 @@
       <c r="J55" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="K55" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="5">
@@ -2924,16 +2966,16 @@
       <c r="J56" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K56" s="22" t="s">
+      <c r="K56" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="22"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="5">
@@ -2956,30 +2998,36 @@
         <v>3.7509999999999999</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" ref="G57:G62" si="3">D57/F57/10</f>
+        <f t="shared" ref="G57:G63" si="3">D57/F57/10</f>
         <v>1.0663822980538522</v>
       </c>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I57" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K57" s="22" t="s">
+      <c r="K57" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22"/>
-      <c r="N57" s="22"/>
-      <c r="O57" s="22"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="22"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B58" s="8">
+        <v>0.58888888888888891</v>
+      </c>
       <c r="C58" s="4" t="s">
         <v>82</v>
       </c>
@@ -2997,25 +3045,33 @@
         <f t="shared" si="3"/>
         <v>1.6396802623488422</v>
       </c>
-      <c r="H58" s="4"/>
+      <c r="H58" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I58" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
+      <c r="K58" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
     </row>
     <row r="59" spans="1:18">
-      <c r="A59" s="5"/>
-      <c r="B59" s="8"/>
+      <c r="A59" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B59" s="8">
+        <v>0.60277777777777775</v>
+      </c>
       <c r="C59" s="4" t="s">
         <v>82</v>
       </c>
@@ -3033,197 +3089,230 @@
         <f t="shared" si="3"/>
         <v>2.1290185224611453</v>
       </c>
-      <c r="H59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="I59" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
+      <c r="K59" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" s="5"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B60" s="8">
+        <v>0.6166666666666667</v>
+      </c>
       <c r="C60" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="4">
+        <v>30</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F60" s="4">
+        <f>F59</f>
+        <v>1.4091</v>
+      </c>
+      <c r="G60" s="4">
+        <f t="shared" si="3"/>
+        <v>2.1290185224611453</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K60" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B61" s="8">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="4">
         <v>20</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E61" s="4">
         <v>0.65</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F61" s="4">
         <f>F28</f>
         <v>0.65969999999999995</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G61" s="4">
         <f t="shared" si="3"/>
         <v>3.031681067151736</v>
       </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4" t="s">
+      <c r="H61" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="22"/>
-    </row>
-    <row r="61" spans="1:18">
-      <c r="A61" s="5"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="4" t="s">
+      <c r="K61" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B62" s="8">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <v>80</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E62" s="4">
         <v>1.25</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F62" s="4">
         <f>F58</f>
         <v>2.4394999999999998</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G62" s="4">
         <f t="shared" si="3"/>
         <v>3.2793605246976845</v>
       </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4" t="s">
+      <c r="H62" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K61" s="22"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="22"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
-      <c r="R61" s="22"/>
-    </row>
-    <row r="62" spans="1:18">
-      <c r="C62" s="4" t="s">
+      <c r="K62" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B63" s="8">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <v>60</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E63" s="4">
         <v>0.95</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F63" s="4">
         <f>F59</f>
         <v>1.4091</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G63" s="4">
         <f t="shared" si="3"/>
         <v>4.2580370449222906</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4" t="s">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-    </row>
-    <row r="63" spans="1:18">
-      <c r="A63" s="5"/>
-      <c r="B63" s="8"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
+      <c r="K63" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="5"/>
-      <c r="B64" s="8">
+      <c r="B64" s="8"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" s="5"/>
+      <c r="B65" s="8">
         <v>0.50347222222222221</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="K65" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="K61:R61"/>
-    <mergeCell ref="K62:R62"/>
-    <mergeCell ref="K63:R63"/>
-    <mergeCell ref="K64:R64"/>
-    <mergeCell ref="K56:R56"/>
-    <mergeCell ref="K55:R55"/>
-    <mergeCell ref="K57:R57"/>
-    <mergeCell ref="K58:R58"/>
-    <mergeCell ref="K59:R59"/>
-    <mergeCell ref="K60:R60"/>
-    <mergeCell ref="K27:R27"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="K29:R29"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K31:R31"/>
-    <mergeCell ref="K34:R34"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="K16:R16"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="K23:R23"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="K20:R20"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="T1:U2"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="A1:R3"/>
-    <mergeCell ref="A5:J6"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="S26:U40"/>
-    <mergeCell ref="T8:U9"/>
-    <mergeCell ref="K32:R32"/>
-    <mergeCell ref="K33:R33"/>
+  <mergeCells count="54">
     <mergeCell ref="K35:R35"/>
     <mergeCell ref="K36:R36"/>
     <mergeCell ref="K18:R18"/>
@@ -3238,6 +3327,46 @@
     <mergeCell ref="K47:R47"/>
     <mergeCell ref="K48:R48"/>
     <mergeCell ref="K49:R49"/>
+    <mergeCell ref="T1:U2"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="A1:R3"/>
+    <mergeCell ref="A5:J6"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="T8:U9"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K31:R31"/>
+    <mergeCell ref="K34:R34"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="K32:R32"/>
+    <mergeCell ref="K33:R33"/>
+    <mergeCell ref="S26:V40"/>
+    <mergeCell ref="K62:R62"/>
+    <mergeCell ref="K63:R63"/>
+    <mergeCell ref="K64:R64"/>
+    <mergeCell ref="K65:R65"/>
+    <mergeCell ref="K56:R56"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K57:R57"/>
+    <mergeCell ref="K58:R58"/>
+    <mergeCell ref="K59:R59"/>
+    <mergeCell ref="K61:R61"/>
+    <mergeCell ref="K27:R27"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="K29:R29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Moved Main_WaveData -> Main_AttnData
</commit_message>
<xml_diff>
--- a/Docs/CITEPH/TestNotes_LB.xlsx
+++ b/Docs/CITEPH/TestNotes_LB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
   <si>
     <t xml:space="preserve">Oceanide/CITEPH July 2013 </t>
   </si>
@@ -277,6 +277,33 @@
   </si>
   <si>
     <t xml:space="preserve">Similar to prev expt. More pitching. Slight scattering from linear waves. Again, eventually corrupted by non-lin waves from WM. </t>
+  </si>
+  <si>
+    <t>More of the same. Pronounced scattering with from and rear lobes -&gt; does this come from the pitching? Close to onset of OW.</t>
+  </si>
+  <si>
+    <t>Repeat of prev test but with 100 periods to help calculate drift</t>
+  </si>
+  <si>
+    <t>Scatterered waves significant (may be picked up by probes). OW beginning (100mm at front of floe). Is the `high fre' appearance of circ waves due to phase mismatch of angular modes?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OW gradually builds up from WM side of floe till front of floe is weighted down &amp; OW flow  begins. Scattering strong - partic ref (from OW?). </t>
+  </si>
+  <si>
+    <t>OW from front &amp; back. Motion less `smooth' than other prev tests (OW or higher amp???). Circ scat waves significant.</t>
+  </si>
+  <si>
+    <t>OW &amp; scattering strong. Is the period of the oscillations that of the wave? OW may perturb this.</t>
+  </si>
+  <si>
+    <t>1 to 1.5</t>
+  </si>
+  <si>
+    <t>1 to 3.5</t>
   </si>
 </sst>
 </file>
@@ -488,35 +515,35 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K42" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57:R57"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -922,72 +949,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="T1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="T1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="17"/>
+      <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
       <c r="T3" t="s">
         <v>7</v>
       </c>
@@ -1004,18 +1031,18 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
       <c r="T5" t="s">
         <v>15</v>
       </c>
@@ -1024,16 +1051,16 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
       <c r="T6" t="s">
         <v>16</v>
       </c>
@@ -1042,22 +1069,22 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="T8" s="17" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="T8" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="17"/>
+      <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:21">
       <c r="T10">
@@ -1098,16 +1125,16 @@
       <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
       <c r="T11">
         <v>0.8</v>
       </c>
@@ -1155,16 +1182,16 @@
       <c r="J13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
       <c r="T13">
         <v>1.1000000000000001</v>
       </c>
@@ -1195,8 +1222,8 @@
         <f t="shared" ref="G14:G31" si="0">D14/F14/10</f>
         <v>2.0016012810248198</v>
       </c>
-      <c r="H14" s="1">
-        <v>3.5</v>
+      <c r="H14" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>22</v>
@@ -1204,16 +1231,16 @@
       <c r="J14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
       <c r="T14">
         <v>1.25</v>
       </c>
@@ -1244,8 +1271,8 @@
         <f t="shared" si="0"/>
         <v>4.0032025620496396</v>
       </c>
-      <c r="H15" s="1">
-        <v>1.5</v>
+      <c r="H15" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>45</v>
@@ -1253,16 +1280,16 @@
       <c r="J15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
       <c r="T15">
         <v>1.4</v>
       </c>
@@ -1302,16 +1329,16 @@
       <c r="J16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
       <c r="T16">
         <v>1.55</v>
       </c>
@@ -1319,7 +1346,7 @@
         <v>3.7509999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" s="5">
         <v>41478</v>
       </c>
@@ -1351,16 +1378,16 @@
       <c r="J17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
       <c r="T17">
         <v>1.7</v>
       </c>
@@ -1368,7 +1395,7 @@
         <v>4.5122</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" s="5">
         <v>41479</v>
       </c>
@@ -1401,16 +1428,16 @@
       <c r="J18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
       <c r="T18">
         <v>1.85</v>
       </c>
@@ -1418,7 +1445,7 @@
         <v>5.3436000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" s="5">
         <v>41479</v>
       </c>
@@ -1451,16 +1478,16 @@
       <c r="J19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
       <c r="T19">
         <v>2</v>
       </c>
@@ -1468,7 +1495,7 @@
         <v>6.2451999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="A20" s="5">
         <v>41479</v>
       </c>
@@ -1501,18 +1528,18 @@
       <c r="J20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="5">
         <v>41479</v>
       </c>
@@ -1545,18 +1572,18 @@
       <c r="J21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="5">
         <v>41479</v>
       </c>
@@ -1589,18 +1616,18 @@
       <c r="J22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="5">
         <v>41479</v>
       </c>
@@ -1633,18 +1660,18 @@
       <c r="J23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="5">
         <v>41479</v>
       </c>
@@ -1677,18 +1704,18 @@
       <c r="J24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="5">
         <v>41479</v>
       </c>
@@ -1721,18 +1748,18 @@
       <c r="J25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="5">
         <v>41479</v>
       </c>
@@ -1765,23 +1792,24 @@
       <c r="J26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K26" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="21" t="s">
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="5">
         <v>41479</v>
       </c>
@@ -1814,21 +1842,22 @@
       <c r="J27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="5">
         <v>41480</v>
       </c>
@@ -1861,21 +1890,22 @@
       <c r="J28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="5">
         <v>41480</v>
       </c>
@@ -1908,21 +1938,22 @@
       <c r="J29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="16" t="s">
+      <c r="K29" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="5">
         <v>41480</v>
       </c>
@@ -1955,21 +1986,22 @@
       <c r="J30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="16" t="s">
+      <c r="K30" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="21"/>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="5">
         <v>41480</v>
       </c>
@@ -2002,21 +2034,22 @@
       <c r="J31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="5">
         <v>41480</v>
       </c>
@@ -2049,21 +2082,22 @@
       <c r="J32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="16" t="s">
+      <c r="K32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="5">
         <v>41480</v>
       </c>
@@ -2096,21 +2130,22 @@
       <c r="J33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K33" s="16" t="s">
+      <c r="K33" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="5">
         <v>41480</v>
       </c>
@@ -2143,21 +2178,22 @@
       <c r="J34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="5">
         <v>41480</v>
       </c>
@@ -2190,21 +2226,22 @@
       <c r="J35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="16" t="s">
+      <c r="K35" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="5">
         <v>41480</v>
       </c>
@@ -2237,21 +2274,22 @@
       <c r="J36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="16" t="s">
+      <c r="K36" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2270,16 +2308,17 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-    </row>
-    <row r="38" spans="1:21" ht="15" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="12"/>
+    </row>
+    <row r="38" spans="1:22" ht="15" customHeight="1">
+      <c r="A38" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2295,14 +2334,15 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
-    </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+    </row>
+    <row r="39" spans="1:22" ht="15" customHeight="1">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2318,11 +2358,12 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2341,11 +2382,12 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
@@ -2376,18 +2418,18 @@
       <c r="J41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="5">
         <v>41479</v>
       </c>
@@ -2420,18 +2462,18 @@
       <c r="J42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K42" s="16" t="s">
+      <c r="K42" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" s="5">
         <v>41479</v>
       </c>
@@ -2464,18 +2506,18 @@
       <c r="J43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="16" t="s">
+      <c r="K43" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="5">
         <v>41479</v>
       </c>
@@ -2508,18 +2550,18 @@
       <c r="J44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K44" s="16" t="s">
+      <c r="K44" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="5">
         <v>41479</v>
       </c>
@@ -2552,18 +2594,18 @@
       <c r="J45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K45" s="16" t="s">
+      <c r="K45" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16"/>
-      <c r="R45" s="16"/>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" s="5">
         <v>41480</v>
       </c>
@@ -2596,18 +2638,18 @@
       <c r="J46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K46" s="16" t="s">
+      <c r="K46" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="L46" s="16"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="16"/>
-      <c r="O46" s="16"/>
-      <c r="P46" s="16"/>
-      <c r="Q46" s="16"/>
-      <c r="R46" s="16"/>
-    </row>
-    <row r="47" spans="1:21">
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="5">
         <v>41480</v>
       </c>
@@ -2640,18 +2682,18 @@
       <c r="J47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K47" s="16" t="s">
+      <c r="K47" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
-    </row>
-    <row r="48" spans="1:21">
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="5">
         <v>41480</v>
       </c>
@@ -2676,16 +2718,16 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="16" t="s">
+      <c r="K48" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="5">
@@ -2712,16 +2754,16 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="16" t="s">
+      <c r="K49" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="16"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
@@ -2744,11 +2786,11 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2766,9 +2808,9 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2836,16 +2878,16 @@
       <c r="J54" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K54" s="14" t="s">
+      <c r="K54" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="22"/>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="5">
@@ -2880,16 +2922,16 @@
       <c r="J55" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="K55" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="5">
@@ -2924,16 +2966,16 @@
       <c r="J56" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K56" s="22" t="s">
+      <c r="K56" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="22"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="5">
@@ -2956,30 +2998,36 @@
         <v>3.7509999999999999</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" ref="G57:G62" si="3">D57/F57/10</f>
+        <f t="shared" ref="G57:G63" si="3">D57/F57/10</f>
         <v>1.0663822980538522</v>
       </c>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I57" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K57" s="22" t="s">
+      <c r="K57" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22"/>
-      <c r="N57" s="22"/>
-      <c r="O57" s="22"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="22"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B58" s="8">
+        <v>0.58888888888888891</v>
+      </c>
       <c r="C58" s="4" t="s">
         <v>82</v>
       </c>
@@ -2997,25 +3045,33 @@
         <f t="shared" si="3"/>
         <v>1.6396802623488422</v>
       </c>
-      <c r="H58" s="4"/>
+      <c r="H58" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I58" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
+      <c r="K58" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
     </row>
     <row r="59" spans="1:18">
-      <c r="A59" s="5"/>
-      <c r="B59" s="8"/>
+      <c r="A59" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B59" s="8">
+        <v>0.60277777777777775</v>
+      </c>
       <c r="C59" s="4" t="s">
         <v>82</v>
       </c>
@@ -3033,197 +3089,230 @@
         <f t="shared" si="3"/>
         <v>2.1290185224611453</v>
       </c>
-      <c r="H59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="I59" s="4" t="s">
         <v>82</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
+      <c r="K59" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" s="5"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B60" s="8">
+        <v>0.6166666666666667</v>
+      </c>
       <c r="C60" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="4">
+        <v>30</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F60" s="4">
+        <f>F59</f>
+        <v>1.4091</v>
+      </c>
+      <c r="G60" s="4">
+        <f t="shared" si="3"/>
+        <v>2.1290185224611453</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K60" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B61" s="8">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="4">
         <v>20</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E61" s="4">
         <v>0.65</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F61" s="4">
         <f>F28</f>
         <v>0.65969999999999995</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G61" s="4">
         <f t="shared" si="3"/>
         <v>3.031681067151736</v>
       </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4" t="s">
+      <c r="H61" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="22"/>
-    </row>
-    <row r="61" spans="1:18">
-      <c r="A61" s="5"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="4" t="s">
+      <c r="K61" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B62" s="8">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <v>80</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E62" s="4">
         <v>1.25</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F62" s="4">
         <f>F58</f>
         <v>2.4394999999999998</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G62" s="4">
         <f t="shared" si="3"/>
         <v>3.2793605246976845</v>
       </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4" t="s">
+      <c r="H62" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K61" s="22"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="22"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
-      <c r="R61" s="22"/>
-    </row>
-    <row r="62" spans="1:18">
-      <c r="C62" s="4" t="s">
+      <c r="K62" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" s="5">
+        <v>41488</v>
+      </c>
+      <c r="B63" s="8">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <v>60</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E63" s="4">
         <v>0.95</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F63" s="4">
         <f>F59</f>
         <v>1.4091</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G63" s="4">
         <f t="shared" si="3"/>
         <v>4.2580370449222906</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4" t="s">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-    </row>
-    <row r="63" spans="1:18">
-      <c r="A63" s="5"/>
-      <c r="B63" s="8"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
+      <c r="K63" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="5"/>
-      <c r="B64" s="8">
+      <c r="B64" s="8"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" s="5"/>
+      <c r="B65" s="8">
         <v>0.50347222222222221</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="K65" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="K61:R61"/>
-    <mergeCell ref="K62:R62"/>
-    <mergeCell ref="K63:R63"/>
-    <mergeCell ref="K64:R64"/>
-    <mergeCell ref="K56:R56"/>
-    <mergeCell ref="K55:R55"/>
-    <mergeCell ref="K57:R57"/>
-    <mergeCell ref="K58:R58"/>
-    <mergeCell ref="K59:R59"/>
-    <mergeCell ref="K60:R60"/>
-    <mergeCell ref="K27:R27"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="K29:R29"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K31:R31"/>
-    <mergeCell ref="K34:R34"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="K16:R16"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="K23:R23"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="K20:R20"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="T1:U2"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="A1:R3"/>
-    <mergeCell ref="A5:J6"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="S26:U40"/>
-    <mergeCell ref="T8:U9"/>
-    <mergeCell ref="K32:R32"/>
-    <mergeCell ref="K33:R33"/>
+  <mergeCells count="54">
     <mergeCell ref="K35:R35"/>
     <mergeCell ref="K36:R36"/>
     <mergeCell ref="K18:R18"/>
@@ -3238,6 +3327,46 @@
     <mergeCell ref="K47:R47"/>
     <mergeCell ref="K48:R48"/>
     <mergeCell ref="K49:R49"/>
+    <mergeCell ref="T1:U2"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="A1:R3"/>
+    <mergeCell ref="A5:J6"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="T8:U9"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K31:R31"/>
+    <mergeCell ref="K34:R34"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="K32:R32"/>
+    <mergeCell ref="K33:R33"/>
+    <mergeCell ref="S26:V40"/>
+    <mergeCell ref="K62:R62"/>
+    <mergeCell ref="K63:R63"/>
+    <mergeCell ref="K64:R64"/>
+    <mergeCell ref="K65:R65"/>
+    <mergeCell ref="K56:R56"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K57:R57"/>
+    <mergeCell ref="K58:R58"/>
+    <mergeCell ref="K59:R59"/>
+    <mergeCell ref="K61:R61"/>
+    <mergeCell ref="K27:R27"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="K29:R29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>